<commit_message>
Added mesg queue sizes and seconds scaling factor
</commit_message>
<xml_diff>
--- a/iot_config.xlsx
+++ b/iot_config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t xml:space="preserve">Description: This is the start of the configuration details:  </t>
   </si>
@@ -85,6 +85,42 @@
   </si>
   <si>
     <t>Contents: What needs to be in here? Well, everything that the user wants as a configuration.  In addition, system configuration that the user will not have control over.</t>
+  </si>
+  <si>
+    <t>MQTT Server IP</t>
+  </si>
+  <si>
+    <t>IP to which our embedded client will connect</t>
+  </si>
+  <si>
+    <t>ip</t>
+  </si>
+  <si>
+    <t>Message Queue Scoppiare</t>
+  </si>
+  <si>
+    <t>Number and size of queues for MetOceon Protocol</t>
+  </si>
+  <si>
+    <t>16 Queues</t>
+  </si>
+  <si>
+    <t>Message Queues Ethernet</t>
+  </si>
+  <si>
+    <t>Number and size of queues for ethernet driver</t>
+  </si>
+  <si>
+    <t>Message Queues Scripting</t>
+  </si>
+  <si>
+    <t>Number and size of queues for script transfer</t>
+  </si>
+  <si>
+    <t>For timeouts, the 6 bit seconds feils has a multiplier factor applied, one second = 5 seconds</t>
+  </si>
+  <si>
+    <t>Seconds Scaling Factor</t>
   </si>
 </sst>
 </file>
@@ -285,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -317,6 +353,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -327,6 +368,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -365,17 +412,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,9 +697,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="10" max="10" width="10.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
@@ -673,52 +717,52 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="23"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="31"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B7" s="24"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="26"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="31"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="27"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="29"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="34"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="19"/>
+      <c r="C11" s="22"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
@@ -759,15 +803,21 @@
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="17"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="9"/>
+      <c r="B13" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="36"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
@@ -777,9 +827,9 @@
       <c r="Q13" s="9"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="6"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -795,9 +845,9 @@
       <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -813,9 +863,9 @@
       <c r="Q15" s="9"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="22"/>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -1047,28 +1097,28 @@
       <c r="Q28" s="9"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="37"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="37"/>
-      <c r="Q29" s="37"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
     </row>
     <row r="31" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="19"/>
+      <c r="C31" s="22"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
@@ -1109,18 +1159,18 @@
       </c>
     </row>
     <row r="33" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="20" t="s">
+      <c r="C33" s="36"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="34"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="25"/>
       <c r="J33" s="9" t="s">
         <v>12</v>
       </c>
@@ -1141,16 +1191,24 @@
       <c r="Q33" s="9"/>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B34" s="17"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
+      <c r="B34" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="21"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K34" s="9">
+        <v>340</v>
+      </c>
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
@@ -1159,16 +1217,24 @@
       <c r="Q34" s="9"/>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="6"/>
+      <c r="B35" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="21"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="8"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
+      <c r="J35" s="9">
+        <v>2</v>
+      </c>
+      <c r="K35" s="9">
+        <v>1500</v>
+      </c>
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="9"/>
@@ -1177,16 +1243,24 @@
       <c r="Q35" s="9"/>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="6"/>
+      <c r="B36" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="21"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="8"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
+      <c r="J36" s="9">
+        <v>8</v>
+      </c>
+      <c r="K36" s="9">
+        <v>256</v>
+      </c>
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
@@ -1195,15 +1269,21 @@
       <c r="Q36" s="9"/>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B37" s="2"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="9"/>
+      <c r="B37" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="21"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="9">
+        <v>5</v>
+      </c>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
@@ -1411,7 +1491,9 @@
       <c r="Q48" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="16">
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:I37"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="E33:I33"/>
     <mergeCell ref="B5:I8"/>
@@ -1425,6 +1507,7 @@
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="E13:I13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E34:I34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>